<commit_message>
API & Web Test Enhanced for Client Demo & Mobile base Started.
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -10,8 +10,13 @@
   <sheets>
     <sheet name="SuiteDetails" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="UserDetails" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="ProductDetails" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="CardDetails" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="MyInfoDetails" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="ProductDetails" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="CardDetails" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="APIDetails" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="HeaderDetails" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="RequestPayloadDetails" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="ResponseDetails" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SuiteDetails!$A$1:$M$3</definedName>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="109">
   <si>
     <t xml:space="preserve">P_Key</t>
   </si>
@@ -85,10 +90,10 @@
     <t xml:space="preserve">loginValid</t>
   </si>
   <si>
-    <t xml:space="preserve">UserDetails~ValidUser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_1</t>
+    <t xml:space="preserve">UserDetails~ValidUser,MyInfoDetails~UpdateValid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_WEB_1</t>
   </si>
   <si>
     <t xml:space="preserve">Web</t>
@@ -97,28 +102,85 @@
     <t xml:space="preserve">SmokeSuite</t>
   </si>
   <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login Invalid – User details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loginInvalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserDetails~InvalidUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_WEB_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apiLoginValid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserDetails~APIValidUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_API_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apiLoginInvalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_API_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobileLoginValid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserDetails~MobileValidUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_MOB_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Login Invalid – User details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loginInvalid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserDetails~InvalidUser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">mobileLogi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nInvalid</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_MOB_2</t>
   </si>
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
   <si>
-    <t xml:space="preserve">Email</t>
+    <t xml:space="preserve">Username</t>
   </si>
   <si>
     <t xml:space="preserve">Password</t>
@@ -142,6 +204,66 @@
     <t xml:space="preserve">InvalidPassword</t>
   </si>
   <si>
+    <t xml:space="preserve">APIValidUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MobileValidUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MiddleName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EmployeeID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OtherID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DLNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSNNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SINNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nationality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaritalStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smoker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UpdateValid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saudi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
     <t xml:space="preserve">ProductName</t>
   </si>
   <si>
@@ -173,6 +295,114 @@
   </si>
   <si>
     <t xml:space="preserve">1234-1234-1234-1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTTPMethod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HeaderReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RequestURL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EndPoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RequestPayloadReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResponseReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content_Type_application_json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/auth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login_Request_Payload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login_Success</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoginInvalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login_Failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RequestHeaders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "Content-Type": "application/json"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RequestPayload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "password": "{password}",
+  "username": "{username}"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExpectedResponseStatusCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExpectedResponseStatusMessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExpectedSchema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExpectedResponsePayload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "$schema": "http://json-schema.org/draft-04/schema#",
+  "type": "object",
+  "properties": {
+    "token": {
+      "type": "string"
+    }
+  },
+  "required": [
+    "token"
+  ]
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"token":"{api_token}"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "$schema": "http://json-schema.org/draft-04/schema#",
+  "type": "object",
+  "properties": {
+    "reason": {
+      "type": "string"
+    }
+  },
+  "required": [
+    "reason"
+  ]
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"reason":"Bad credentials"}</t>
   </si>
 </sst>
 </file>
@@ -182,7 +412,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -237,6 +467,26 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCE93D8"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -270,7 +520,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -292,6 +542,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -321,7 +578,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -374,6 +631,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -386,7 +647,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -446,7 +719,11 @@
     </dxf>
     <dxf>
       <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
         <color rgb="FF9C0006"/>
+        <sz val="11"/>
       </font>
       <fill>
         <patternFill>
@@ -495,7 +772,7 @@
       <rgbColor rgb="FFFFD966"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFCE93D8"/>
       <rgbColor rgb="FFFFC7CE"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -527,17 +804,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M6" activeCellId="0" sqref="M6"/>
+      <selection pane="bottomRight" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="19.4"/>
@@ -545,7 +822,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="18.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="35.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="10.01"/>
@@ -664,7 +941,9 @@
       <c r="L3" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="M3" s="12"/>
+      <c r="M3" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="n">
@@ -674,17 +953,17 @@
         <v>16</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>21</v>
@@ -693,7 +972,7 @@
         <v>22</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="K4" s="12" t="n">
         <v>1</v>
@@ -701,12 +980,160 @@
       <c r="L4" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="M4" s="12"/>
+      <c r="M4" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F5" s="12"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A5" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="12" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="12" t="n">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M3"/>
   <conditionalFormatting sqref="E1:E2 F1">
@@ -731,47 +1158,69 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="9.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="30.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="14.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="14.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="14.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>31</v>
+      <c r="A1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>34</v>
+      <c r="A2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>37</v>
+      <c r="A3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -791,6 +1240,112 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="14" t="n">
+        <v>101</v>
+      </c>
+      <c r="F2" s="14" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G2" s="14" t="n">
+        <v>231568645</v>
+      </c>
+      <c r="H2" s="14" t="n">
+        <v>78879</v>
+      </c>
+      <c r="I2" s="14" t="n">
+        <v>5565665456</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -799,63 +1354,63 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="9.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="8.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>39</v>
+      <c r="A1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="13" t="n">
+      <c r="A2" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="14" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="13" t="n">
+      <c r="A3" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="14" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="13" t="n">
+      <c r="A4" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="14" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="13" t="n">
+      <c r="A5" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="14" t="n">
         <v>2</v>
       </c>
     </row>
@@ -871,7 +1426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -879,35 +1434,35 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="9.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="19.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="4.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="19.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="4.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>46</v>
+      <c r="A1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="13" t="n">
+      <c r="A2" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="14" t="n">
         <v>234</v>
       </c>
     </row>
@@ -921,4 +1476,266 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="25.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="11.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="22.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="14" width="17.38"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="25.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="29.63"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="19.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="13.8"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="12.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="26.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="28.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="23.23"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="172.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="172.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test Dependent data - Pushed
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -120,19 +120,19 @@
     <t xml:space="preserve">TC_WEB_2</t>
   </si>
   <si>
+    <t xml:space="preserve">apiLoginValid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserDetails~APIValidUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_API_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API</t>
+  </si>
+  <si>
     <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">apiLoginValid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserDetails~APIValidUser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_API_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">API</t>
   </si>
   <si>
     <t xml:space="preserve">apiLoginInvalid</t>
@@ -783,7 +783,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J5" activeCellId="0" sqref="J5:J8"/>
+      <selection pane="bottomRight" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -944,7 +944,7 @@
         <v>22</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K4" s="12" t="n">
         <v>1</v>
@@ -968,22 +968,22 @@
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="G5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="H5" s="12" t="s">
         <v>32</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K5" s="12" t="n">
         <v>1</v>
@@ -1016,13 +1016,13 @@
         <v>35</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K6" s="12" t="n">
         <v>1</v>
@@ -1061,7 +1061,7 @@
         <v>22</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K7" s="12" t="n">
         <v>1</v>
@@ -1097,7 +1097,7 @@
         <v>22</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K8" s="12" t="n">
         <v>1</v>
@@ -1130,7 +1130,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="J5:J8 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="J5:J8 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1321,7 +1321,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="J5:J8 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1406,7 +1406,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="J5:J8 C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1458,7 +1458,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="1" sqref="J5:J8 G3"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1554,7 +1554,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="J5:J8 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1598,7 +1598,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J5:J8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1642,7 +1642,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="J5:J8 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
committing mobile test case1 loginvalid
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOHAMMAD.RAFI\TestAutomation\agichildProject\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOHAMMAD.RAFI\TestAutomation\projects\kabi\agi_KabiProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0E521F-1C8C-4407-AE9C-69C214243A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8018B2E-426B-49A3-BD32-5A07E6598371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -990,10 +990,10 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
@@ -1301,7 +1301,7 @@
         <v>22</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K8" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
login valid and invalid scripts update
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOHAMMAD.RAFI\TestAutomation\projects\kabi\agi_KabiProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8018B2E-426B-49A3-BD32-5A07E6598371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4BE19A-8882-4976-951E-A63D68A461FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SuiteDetails" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="101">
   <si>
     <t>P_Key</t>
   </si>
@@ -146,61 +146,16 @@
     <t>TC_API_2</t>
   </si>
   <si>
-    <t>mobileLoginValid</t>
-  </si>
-  <si>
-    <t>UserDetails~MobileValidUser</t>
-  </si>
-  <si>
     <t>TC_MOB_1</t>
   </si>
   <si>
     <t>Mobile</t>
   </si>
   <si>
-    <t>mobileLoginInvalid</t>
-  </si>
-  <si>
     <t>TC_MOB_2</t>
   </si>
   <si>
     <t>Reference</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>ValidUser</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>InvalidUser</t>
-  </si>
-  <si>
-    <t>InvalidUsername</t>
-  </si>
-  <si>
-    <t>InvalidPassword</t>
-  </si>
-  <si>
-    <t>APIValidUser</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>password123</t>
-  </si>
-  <si>
-    <t>MobileValidUser</t>
   </si>
   <si>
     <t>FirstName</t>
@@ -391,12 +346,33 @@
   <si>
     <t>{"reason":"Bad credentials"}</t>
   </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>Driverid</t>
+  </si>
+  <si>
+    <t>loginValidDriverID</t>
+  </si>
+  <si>
+    <t>loginInvalidDriverID</t>
+  </si>
+  <si>
+    <t>InvalidUser</t>
+  </si>
+  <si>
+    <t>UserDetails~ValidUser</t>
+  </si>
+  <si>
+    <t>ValidUser</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -434,13 +410,6 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCE93D8"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
       <charset val="1"/>
     </font>
     <font>
@@ -564,11 +533,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -989,21 +960,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.08984375" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.36328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="22.36328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.90625" style="2" customWidth="1"/>
     <col min="5" max="5" width="18.26953125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="35.26953125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="44.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.36328125" style="2" customWidth="1"/>
     <col min="8" max="8" width="10.6328125" style="2" customWidth="1"/>
     <col min="9" max="9" width="11.6328125" style="2" customWidth="1"/>
@@ -1014,7 +985,7 @@
     <col min="14" max="16384" width="11.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1055,7 +1026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18">
+    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.5">
       <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
@@ -1088,7 +1059,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17">
+    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.5">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -1126,7 +1097,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17">
+    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.5">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -1164,7 +1135,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17">
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.5">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -1202,7 +1173,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17">
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.5">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -1240,7 +1211,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17">
+    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.5">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -1251,16 +1222,16 @@
         <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>22</v>
@@ -1275,7 +1246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17">
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.5">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -1286,16 +1257,16 @@
         <v>25</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>22</v>
@@ -1316,78 +1287,56 @@
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" customWidth="1"/>
     <col min="3" max="3" width="14.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>100</v>
+      </c>
+      <c r="B2" s="16">
+        <v>3114791</v>
+      </c>
+      <c r="C2" s="16">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
+        <v>98</v>
+      </c>
+      <c r="B3" s="16">
+        <v>1234567</v>
+      </c>
+      <c r="C3" s="16">
+        <v>123456</v>
       </c>
     </row>
   </sheetData>
@@ -1408,61 +1357,61 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>57</v>
-      </c>
       <c r="E1" s="13" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="E2">
         <v>101</v>
@@ -1480,13 +1429,13 @@
         <v>5565665456</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="L2" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="M2" t="s">
         <v>23</v>
@@ -1510,63 +1459,63 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.54296875" customWidth="1"/>
     <col min="2" max="2" width="12.81640625" customWidth="1"/>
     <col min="3" max="3" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1586,30 +1535,30 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.54296875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="4.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C2">
         <v>234</v>
@@ -1633,7 +1582,7 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.54296875" customWidth="1"/>
     <col min="2" max="2" width="12.26953125" customWidth="1"/>
@@ -1644,67 +1593,67 @@
     <col min="7" max="7" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1725,26 +1674,26 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.90625" customWidth="1"/>
     <col min="2" max="2" width="29.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="58">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>97</v>
+        <v>75</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1763,26 +1712,26 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.90625" customWidth="1"/>
     <col min="2" max="2" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="87">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>99</v>
+        <v>77</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1803,7 +1752,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.6328125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -1812,51 +1761,51 @@
     <col min="5" max="5" width="23.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="232">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" t="s">
         <v>93</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="E2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="232">
-      <c r="A3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated changes of the project
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOHAMMAD.RAFI\TestAutomation\projects\kabi\agi_KabiProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8971A56D-BAD3-40EC-A9D1-943225AAC5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8DDFA6-6CB1-426B-8E8F-876070A671CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -122,9 +122,6 @@
     <t>TC_WEB_2</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>apiLoginValid</t>
   </si>
   <si>
@@ -412,6 +409,9 @@
   </si>
   <si>
     <t>SanitySuite</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -597,6 +597,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1019,20 +1028,20 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" style="23" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" style="2" bestFit="1" customWidth="1"/>
@@ -1050,7 +1059,7 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -1089,9 +1098,9 @@
         <v>13</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="8"/>
+        <v>71</v>
+      </c>
+      <c r="C2" s="22"/>
       <c r="D2" s="8"/>
       <c r="E2" s="9" t="s">
         <v>14</v>
@@ -1117,14 +1126,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="23" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -1142,8 +1151,8 @@
       <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>28</v>
+      <c r="J3" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="K3" s="3">
         <v>1</v>
@@ -1155,14 +1164,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="23" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1180,8 +1189,8 @@
       <c r="I4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>28</v>
+      <c r="J4" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="K4" s="3">
         <v>1</v>
@@ -1193,33 +1202,33 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="23" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>28</v>
+      <c r="J5" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="K5" s="3">
         <v>1</v>
@@ -1231,33 +1240,33 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="23" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>28</v>
+      <c r="J6" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="K6" s="3">
         <v>1</v>
@@ -1276,26 +1285,26 @@
       <c r="B7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>104</v>
+      <c r="C7" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G7" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>36</v>
-      </c>
       <c r="I7" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>22</v>
@@ -1314,26 +1323,26 @@
       <c r="B8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>105</v>
+      <c r="C8" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F8" s="18" t="s">
         <v>26</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J8" s="20" t="s">
         <v>22</v>
@@ -1350,28 +1359,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="18" t="s">
         <v>111</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>112</v>
       </c>
       <c r="J9" s="20" t="s">
         <v>22</v>
@@ -1410,21 +1419,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="16">
         <v>3114791</v>
@@ -1435,7 +1444,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="16">
         <v>1234567</v>
@@ -1446,7 +1455,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" s="16">
         <v>3114791</v>
@@ -1478,57 +1487,57 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>49</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
       </c>
       <c r="E2">
         <v>101</v>
@@ -1546,13 +1555,13 @@
         <v>5565665456</v>
       </c>
       <c r="J2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" t="s">
         <v>52</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>53</v>
-      </c>
-      <c r="L2" t="s">
-        <v>54</v>
       </c>
       <c r="M2" t="s">
         <v>22</v>
@@ -1585,21 +1594,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
         <v>57</v>
-      </c>
-      <c r="B2" t="s">
-        <v>58</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1607,10 +1616,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1618,10 +1627,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1629,10 +1638,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1661,21 +1670,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>62</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
         <v>64</v>
-      </c>
-      <c r="B2" t="s">
-        <v>65</v>
       </c>
       <c r="C2">
         <v>234</v>
@@ -1712,65 +1721,65 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>70</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
         <v>72</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>73</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>74</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>75</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>76</v>
-      </c>
-      <c r="G2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
         <v>78</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1799,18 +1808,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1837,18 +1846,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1880,49 +1889,49 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>86</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
         <v>89</v>
-      </c>
-      <c r="E2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
         <v>91</v>
-      </c>
-      <c r="E3" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
publishing results with zephyr cycle timestamp added
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager.xlsx
+++ b/src/test/resources/Run_Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOHAMMAD.RAFI\TestAutomation\projects\kabi\agi_KabiProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97A4964-0F50-49C3-9A65-3B4825B8D90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AFF9AD-F1D7-4C62-A8C4-6008CAC4BEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1028,10 +1028,10 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1307,7 @@
         <v>111</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="K7" s="20">
         <v>1</v>
@@ -1383,7 +1383,7 @@
         <v>111</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
       <c r="K9" s="20">
         <v>1</v>

</xml_diff>